<commit_message>
Revert "ADD MORE VOB"
This reverts commit 0146927cb9b8351999478f687f305631e1ea3435.
</commit_message>
<xml_diff>
--- a/document/Vocabulary.xlsx
+++ b/document/Vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Yao\Documents\GitHub\CSX_RProject_Summer_2018\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D1EA48-6160-4E51-925A-ECD5CC39417B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC7099D-F2A6-4A4F-A248-CDD9F0D7C103}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{FB7D835D-F382-4FB8-B293-6553F62C3CE3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>原文</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,38 +303,6 @@
   </si>
   <si>
     <t>比較運算子</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rows</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>列</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>columns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ordered factors</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>順序型因素向量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>比較級</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>data frame</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -528,8 +496,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{117BF495-3E9E-462D-90BC-6AA772D2DA63}" name="表格1" displayName="表格1" ref="A1:C35" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:C35" xr:uid="{03150B6E-5CEB-46EC-9653-3B038DD3366B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{117BF495-3E9E-462D-90BC-6AA772D2DA63}" name="表格1" displayName="表格1" ref="A1:C31" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:C31" xr:uid="{03150B6E-5CEB-46EC-9653-3B038DD3366B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{270AD1EE-9240-4505-A05C-448242051B3A}" name="原文" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{B49B5F7B-26AD-4D4F-9ABC-239D6B7BA2E3}" name="中文" dataDxfId="2"/>
@@ -848,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB118205-DAC6-4511-A9A6-EB926D361A79}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1182,44 +1150,6 @@
         <v>68</v>
       </c>
       <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>